<commit_message>
Creation of settings window
</commit_message>
<xml_diff>
--- a/WOT.xlsx
+++ b/WOT.xlsx
@@ -8,12 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="КВ2" sheetId="2" r:id="rId1"/>
-    <sheet name="settings" sheetId="3" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Bool">settings!$B:$B</definedName>
+    <definedName name="Bool">Settings!$B:$B</definedName>
     <definedName name="дата">КВ2!$B:$B</definedName>
-    <definedName name="Лист">settings!$A:$A</definedName>
+    <definedName name="Лист">Settings!$A:$A</definedName>
     <definedName name="Оценка">КВ2!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="A2:C7"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>